<commit_message>
Running final trends estimates
</commit_message>
<xml_diff>
--- a/trends/results/table2.xlsx
+++ b/trends/results/table2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>year range</t>
   </si>
@@ -34,19 +34,13 @@
     <t>(0.1)</t>
   </si>
   <si>
-    <t>(0.16)</t>
-  </si>
-  <si>
-    <t>(0.23)</t>
-  </si>
-  <si>
-    <t>(0.27)</t>
-  </si>
-  <si>
-    <t>(0.33)</t>
-  </si>
-  <si>
-    <t>(0.32)</t>
+    <t>(0.15)</t>
+  </si>
+  <si>
+    <t>(0.25)</t>
+  </si>
+  <si>
+    <t>(0.31)</t>
   </si>
   <si>
     <t>(0.03)</t>
@@ -58,13 +52,16 @@
     <t>(0.09)</t>
   </si>
   <si>
+    <t>(0.17)</t>
+  </si>
+  <si>
     <t>(0.22)</t>
   </si>
   <si>
-    <t>(0.17)</t>
-  </si>
-  <si>
-    <t>(0.0)</t>
+    <t>(0.21)</t>
+  </si>
+  <si>
+    <t>(0.00001)</t>
   </si>
 </sst>
 </file>
@@ -456,7 +453,7 @@
         <v>7.1</v>
       </c>
       <c r="E2">
-        <v>0.1825</v>
+        <v>0.182455</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -470,10 +467,10 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -490,7 +487,7 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>0.1673</v>
+        <v>0.167269</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -504,10 +501,10 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -524,7 +521,7 @@
         <v>9.109999999999999</v>
       </c>
       <c r="E6">
-        <v>0.123</v>
+        <v>0.122975</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -538,10 +535,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -558,7 +555,7 @@
         <v>10.61</v>
       </c>
       <c r="E8">
-        <v>0.1012</v>
+        <v>0.101189</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -572,10 +569,10 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -592,7 +589,7 @@
         <v>11.64</v>
       </c>
       <c r="E10">
-        <v>0.09279999999999999</v>
+        <v>0.092802</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -603,13 +600,13 @@
         <v>2007</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -626,7 +623,7 @@
         <v>11.22</v>
       </c>
       <c r="E12">
-        <v>0.09719999999999999</v>
+        <v>0.09722799999999999</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -637,13 +634,13 @@
         <v>2012</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -660,7 +657,7 @@
         <v>9.31</v>
       </c>
       <c r="E14">
-        <v>0.0898</v>
+        <v>0.089807</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -671,13 +668,13 @@
         <v>2017</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
         <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>